<commit_message>
random intermediate objects during fix
</commit_message>
<xml_diff>
--- a/outputs/metric1_track.xlsx
+++ b/outputs/metric1_track.xlsx
@@ -373,10 +373,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>32.78</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
+        <v>31.55</v>
       </c>
     </row>
   </sheetData>
@@ -428,134 +425,110 @@
       <c r="C2">
         <v>89.47</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IN-MZ</t>
+          <t>IN-JH</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mizoram</t>
+          <t>Jharkhand</t>
         </is>
       </c>
       <c r="C3">
-        <v>81.81999999999999</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IN-JH</t>
+          <t>IN-PB</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="C4">
-        <v>75</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
+        <v>63.64</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IN-PB</t>
+          <t>IN-ML</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>Meghalaya</t>
         </is>
       </c>
       <c r="C5">
         <v>63.64</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IN-ML</t>
+          <t>IN-UP</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="C6">
-        <v>63.64</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
+        <v>62.67</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IN-UP</t>
+          <t>IN-MN</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>Manipur</t>
         </is>
       </c>
       <c r="C7">
-        <v>62.67</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IN-MN</t>
+          <t>IN-MZ</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Manipur</t>
+          <t>Mizoram</t>
         </is>
       </c>
       <c r="C8">
-        <v>62.5</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
+        <v>54.55</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IN-NL</t>
+          <t>IN-DD</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Nagaland</t>
+          <t>Daman and Diu</t>
         </is>
       </c>
       <c r="C9">
-        <v>54.55</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10">
@@ -572,171 +545,141 @@
       <c r="C10">
         <v>50</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IN-DD</t>
+          <t>IN-PY</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Daman and Diu</t>
+          <t>Puducherry</t>
         </is>
       </c>
       <c r="C11">
         <v>50</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>IN-PY</t>
+          <t>IN-DL</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Puducherry</t>
+          <t>Delhi</t>
         </is>
       </c>
       <c r="C12">
-        <v>50</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
+        <v>45.45</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>IN-DL</t>
+          <t>IN-AR</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Delhi</t>
+          <t>Arunachal Pradesh</t>
         </is>
       </c>
       <c r="C13">
-        <v>45.45</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>IN-AR</t>
+          <t>IN-NL</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Arunachal Pradesh</t>
+          <t>Nagaland</t>
         </is>
       </c>
       <c r="C14">
-        <v>44</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
+        <v>36.36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IN-OR</t>
+          <t>IN-TS</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>Telangana</t>
         </is>
       </c>
       <c r="C15">
         <v>33.33</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IN-TS</t>
+          <t>IN-MP</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>Madhya Pradesh</t>
         </is>
       </c>
       <c r="C16">
-        <v>33.33</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
+        <v>30.77</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>IN-HR</t>
+          <t>IN-OR</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>Odisha</t>
         </is>
       </c>
       <c r="C17">
-        <v>31.82</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IN-MP</t>
+          <t>IN-JK</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="C18">
-        <v>30.77</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
+        <v>27.27</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IN-JK</t>
+          <t>IN-HR</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="C19">
         <v>27.27</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -752,62 +695,50 @@
       <c r="C20">
         <v>24.24</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IN-HP</t>
+          <t>IN-RJ</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Rajasthan</t>
         </is>
       </c>
       <c r="C21">
-        <v>16.67</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
+        <v>15.15</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>IN-RJ</t>
+          <t>IN-WB</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>West Bengal</t>
         </is>
       </c>
       <c r="C22">
-        <v>15.15</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
+        <v>13.04</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IN-WB</t>
+          <t>IN-HP</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>West Bengal</t>
+          <t>Himachal Pradesh</t>
         </is>
       </c>
       <c r="C23">
-        <v>13.04</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="24">
@@ -824,9 +755,6 @@
       <c r="C24">
         <v>7.41</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -842,9 +770,6 @@
       <c r="C25">
         <v>3.03</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -859,9 +784,6 @@
       </c>
       <c r="C26">
         <v>2.78</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1008,9 +930,6 @@
       <c r="B2">
         <v>91.11</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1019,10 +938,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>47.83</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
+        <v>42.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>